<commit_message>
insert bioBERT.py + correct paths
</commit_message>
<xml_diff>
--- a/Results/mode3_variants.xlsx
+++ b/Results/mode3_variants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stam\Documents\git\Instance-Based-ZSL\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908E6BD7-C569-4115-91E3-8F6A8223D842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B57388-2436-4791-9491-79EF53DB2A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5411B0BC-E70E-46C0-9942-BD79781FD36A}"/>
   </bookViews>
@@ -34,19 +34,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
   <si>
     <t xml:space="preserve"> One-error:</t>
   </si>
   <si>
     <t xml:space="preserve"> Coverage error:</t>
   </si>
+  <si>
+    <t>LSSc(max)</t>
+  </si>
+  <si>
+    <t>RanksSc(max)</t>
+  </si>
+  <si>
+    <t>IBZSL (sum)</t>
+  </si>
+  <si>
+    <t>IBZSL(max) - proposed</t>
+  </si>
+  <si>
+    <t>Algorithms / Seed</t>
+  </si>
+  <si>
+    <t>random_seed = 23</t>
+  </si>
+  <si>
+    <t>random_seed = 24</t>
+  </si>
+  <si>
+    <t>random_seed = 2021</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,13 +78,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,8 +144,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -391,211 +490,1022 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD030C31-F54C-4E3C-9331-0C80AC4300BA}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:27" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="8"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="D2" s="4">
         <v>27.927</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1">
+      <c r="H2" s="4">
         <v>27.975999999999999</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J1">
+      <c r="L2" s="4">
         <v>28.117000000000001</v>
       </c>
-      <c r="O1">
-        <f>_xlfn.STDEV.P(B1,F1,J1)</f>
-        <v>8.0541224778922962E-2</v>
-      </c>
-      <c r="R1">
-        <f>_xlfn.STDEV.P(1,2,3)</f>
-        <v>0.81649658092772603</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="D3" s="4">
         <v>0.89900000000000002</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="H3" s="4">
         <v>0.89900000000000002</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="L3" s="4">
         <v>0.9</v>
       </c>
-      <c r="P2">
-        <f>_xlfn.STDEV.P(C2,G2,K2)</f>
-        <v>4.7140452079103207E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="D5" s="4">
         <v>21.664000000000001</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="H5" s="4">
         <v>21.643000000000001</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J4">
+      <c r="L5" s="4">
         <v>21.757999999999999</v>
       </c>
-      <c r="O4">
-        <f>_xlfn.STDEV.P(B4,F4,J4)</f>
-        <v>5.0002222172840845E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="C6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="4">
         <v>0.81200000000000006</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="H6" s="4">
         <v>0.81399999999999995</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K5">
+      <c r="L6" s="4">
         <v>0.81200000000000006</v>
       </c>
-      <c r="P5">
-        <f>_xlfn.STDEV.P(C5,G5,K5)</f>
-        <v>9.4280904158201189E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7">
+      <c r="D8" s="4">
         <v>10.006</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F7">
+      <c r="H8" s="4">
         <v>9.9450000000000003</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J7">
+      <c r="L8" s="4">
         <v>10.057</v>
       </c>
-      <c r="O7">
-        <f>_xlfn.STDEV.P(B7,F7,J7)</f>
-        <v>4.5784519460427074E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="C9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8">
+      <c r="D9" s="4">
         <v>0.625</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="H9" s="4">
         <v>0.626</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K8">
+      <c r="L9" s="4">
         <v>0.624</v>
       </c>
-      <c r="P8">
-        <f>_xlfn.STDEV.P(C8,G8,K8)</f>
-        <v>8.1649658092772682E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="D11" s="4">
         <v>12.243</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F10">
+      <c r="H11" s="4">
         <v>12.272</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="L11" s="4">
         <v>12.256</v>
       </c>
-      <c r="O10">
-        <f>_xlfn.STDEV.P(B10,F10,J10)</f>
-        <v>1.1860297916438098E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="D12" s="4">
         <v>0.64</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="H12" s="4">
         <v>0.64</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="K11">
+      <c r="L12" s="4">
         <v>0.64</v>
       </c>
-      <c r="P11">
-        <f>_xlfn.STDEV.P(C11,G11,K11)</f>
-        <v>0</v>
-      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>